<commit_message>
Giải thuật GA - Xử lý lỗi
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/PS_CT001_HK4/LichHocKy_PS_CT001_HK4.xlsx
+++ b/timetabling_GA/results/PS_CT001_HK4/LichHocKy_PS_CT001_HK4.xlsx
@@ -22,7 +22,6 @@
     <sheet name="Week_13" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Week_14" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Week_15" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Week_16" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -85,18 +84,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00BDD7EE"/>
+        <bgColor rgb="00BDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FFCCCB"/>
         <bgColor rgb="00FFCCCB"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BDD7EE"/>
-        <bgColor rgb="00BDD7EE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -118,11 +117,44 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -148,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -516,7 +549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,12 +659,12 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
@@ -639,55 +672,295 @@
       </c>
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="8" t="inlineStr">
-        <is>
-          <t>MH005
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="9" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH2
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="9" t="n"/>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH3
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="7" t="inlineStr"/>
+      <c r="F14" s="7" t="inlineStr"/>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="inlineStr"/>
+    </row>
+    <row r="15" ht="60" customHeight="1">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="inlineStr"/>
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="7" t="inlineStr"/>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
         <is>
           <t>MH007
 (Theory)
-Room: LT1
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH1
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="J15" s="7" t="inlineStr"/>
+    </row>
+    <row r="16" ht="60" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH3
 Lecturer: GV003</t>
         </is>
       </c>
-      <c r="I9" s="7" t="inlineStr"/>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10"/>
+      <c r="E16" s="7" t="inlineStr"/>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="inlineStr"/>
+      <c r="H16" s="7" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr"/>
+      <c r="J16" s="7" t="inlineStr"/>
+    </row>
+    <row r="17"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -699,7 +972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,66 +1082,190 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
-    <row r="10"/>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -882,7 +1279,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -992,66 +1389,190 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
-    <row r="10"/>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -1065,7 +1586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,66 +1696,190 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
-    <row r="10"/>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -1248,7 +1893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1358,66 +2003,190 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
-    <row r="10"/>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -1431,7 +2200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1541,66 +2310,190 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
-    <row r="10"/>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -1614,7 +2507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1724,66 +2617,190 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
-    <row r="10"/>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -1791,13 +2808,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1841,7 +2858,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 16 TIMETABLE (26/10/2026 - 01/11/2026)</t>
+          <t>WEEK 2 TIMETABLE (20/07/2026 - 26/07/2026)</t>
         </is>
       </c>
     </row>
@@ -1864,94 +2881,363 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-26/10</t>
+20/07</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-27/10</t>
+21/07</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-28/10</t>
+22/07</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-29/10</t>
+23/07</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-30/10</t>
+24/07</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-31/10</t>
+25/07</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-01/11</t>
+26/07</t>
         </is>
       </c>
     </row>
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
-    <row r="9"/>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="9" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH2
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="9" t="n"/>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH3
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="7" t="inlineStr"/>
+      <c r="F14" s="7" t="inlineStr"/>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="inlineStr"/>
+    </row>
+    <row r="15" ht="60" customHeight="1">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="inlineStr"/>
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="7" t="inlineStr"/>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH1
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="J15" s="7" t="inlineStr"/>
+    </row>
+    <row r="16" ht="60" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH3
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr"/>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="inlineStr"/>
+      <c r="H16" s="7" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr"/>
+      <c r="J16" s="7" t="inlineStr"/>
+    </row>
+    <row r="17"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1995,7 +3281,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 2 TIMETABLE (20/07/2026 - 26/07/2026)</t>
+          <t>WEEK 3 TIMETABLE (27/07/2026 - 02/08/2026)</t>
         </is>
       </c>
     </row>
@@ -2018,43 +3304,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-20/07</t>
+27/07</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-21/07</t>
+28/07</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-22/07</t>
+29/07</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-23/07</t>
+30/07</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-24/07</t>
+31/07</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-25/07</t>
+01/08</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-26/07</t>
+02/08</t>
         </is>
       </c>
     </row>
@@ -2066,14 +3352,57 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr"/>
+      <c r="H8" s="7" t="inlineStr"/>
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="9" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="10" t="inlineStr">
         <is>
           <t>MH007
 (Practice)
@@ -2081,50 +3410,17 @@
 Lecturer: GV003</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
@@ -2134,65 +3430,237 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH005
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH2
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="9" t="n"/>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH3
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr"/>
       <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
-    <row r="12"/>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="7" t="inlineStr"/>
+      <c r="F14" s="7" t="inlineStr"/>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="inlineStr"/>
+    </row>
+    <row r="15" ht="60" customHeight="1">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="inlineStr"/>
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="7" t="inlineStr"/>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH1
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="J15" s="7" t="inlineStr"/>
+    </row>
+    <row r="16" ht="60" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH3
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr"/>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="inlineStr"/>
+      <c r="H16" s="7" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr"/>
+      <c r="J16" s="7" t="inlineStr"/>
+    </row>
+    <row r="17"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2236,7 +3704,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 3 TIMETABLE (27/07/2026 - 02/08/2026)</t>
+          <t>WEEK 4 TIMETABLE (03/08/2026 - 09/08/2026)</t>
         </is>
       </c>
     </row>
@@ -2259,43 +3727,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-27/07</t>
+03/08</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-28/07</t>
+04/08</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-29/07</t>
+05/08</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-30/07</t>
+06/08</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-31/07</t>
+07/08</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-01/08</t>
+08/08</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-02/08</t>
+09/08</t>
         </is>
       </c>
     </row>
@@ -2307,14 +3775,57 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr"/>
+      <c r="H8" s="7" t="inlineStr"/>
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="9" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="10" t="inlineStr">
         <is>
           <t>MH007
 (Practice)
@@ -2322,132 +3833,257 @@
 Lecturer: GV003</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH3
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH005
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH2
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="9" t="n"/>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH3
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH2
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr"/>
       <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
-    <row r="12"/>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="7" t="inlineStr"/>
+      <c r="F14" s="7" t="inlineStr"/>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="inlineStr"/>
+    </row>
+    <row r="15" ht="60" customHeight="1">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="inlineStr"/>
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="7" t="inlineStr"/>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH1
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="J15" s="7" t="inlineStr"/>
+    </row>
+    <row r="16" ht="60" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH3
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr"/>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="inlineStr"/>
+      <c r="H16" s="7" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr"/>
+      <c r="J16" s="7" t="inlineStr"/>
+    </row>
+    <row r="17"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2491,7 +4127,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 4 TIMETABLE (03/08/2026 - 09/08/2026)</t>
+          <t>WEEK 5 TIMETABLE (10/08/2026 - 16/08/2026)</t>
         </is>
       </c>
     </row>
@@ -2514,43 +4150,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-03/08</t>
+10/08</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-04/08</t>
+11/08</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-05/08</t>
+12/08</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-06/08</t>
+13/08</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-07/08</t>
+14/08</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-08/08</t>
+15/08</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-09/08</t>
+16/08</t>
         </is>
       </c>
     </row>
@@ -2562,14 +4198,57 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr"/>
+      <c r="H8" s="7" t="inlineStr"/>
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="9" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="10" t="inlineStr">
         <is>
           <t>MH007
 (Practice)
@@ -2577,50 +4256,17 @@
 Lecturer: GV003</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
@@ -2630,72 +4276,237 @@
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH005
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH2
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="9" t="n"/>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH3
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH1
-Lecturer: GV007</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr"/>
       <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
-    <row r="12"/>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>MH007
+(Practice)
+Room: TH3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="7" t="inlineStr"/>
+      <c r="F14" s="7" t="inlineStr"/>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="inlineStr"/>
+    </row>
+    <row r="15" ht="60" customHeight="1">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="inlineStr"/>
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="7" t="inlineStr"/>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>MH014
+(Practice)
+Room: TH1
+Lecturer: GV006</t>
+        </is>
+      </c>
+      <c r="J15" s="7" t="inlineStr"/>
+    </row>
+    <row r="16" ht="60" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>MH008
+(Practice)
+Room: TH3
+Lecturer: GV003</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr"/>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="inlineStr"/>
+      <c r="H16" s="7" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr"/>
+      <c r="J16" s="7" t="inlineStr"/>
+    </row>
+    <row r="17"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2739,7 +4550,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 5 TIMETABLE (10/08/2026 - 16/08/2026)</t>
+          <t>WEEK 6 TIMETABLE (17/08/2026 - 23/08/2026)</t>
         </is>
       </c>
     </row>
@@ -2762,43 +4573,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-10/08</t>
+17/08</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-11/08</t>
+18/08</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-12/08</t>
+19/08</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-13/08</t>
+20/08</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-14/08</t>
+21/08</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-15/08</t>
+22/08</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-16/08</t>
+23/08</t>
         </is>
       </c>
     </row>
@@ -2810,52 +4621,55 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>MH007
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="F8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
@@ -2863,28 +4677,28 @@
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH1
-Lecturer: GV007</t>
-        </is>
-      </c>
+      <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
@@ -2892,12 +4706,12 @@
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
@@ -2907,15 +4721,15 @@
       <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr"/>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH005
-(Practice)
-Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
     <row r="12" ht="60" customHeight="1">
@@ -2926,7 +4740,7 @@
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C12" s="7" t="n">
@@ -2935,23 +4749,57 @@
       <c r="D12" s="7" t="inlineStr"/>
       <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
         <is>
           <t>MH007
 (Theory)
-Room: LT1
-Lecturer: GV003</t>
+Room: LT2
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
-    <row r="13"/>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -2959,13 +4807,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3009,7 +4857,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 6 TIMETABLE (17/08/2026 - 23/08/2026)</t>
+          <t>WEEK 7 TIMETABLE (24/08/2026 - 30/08/2026)</t>
         </is>
       </c>
     </row>
@@ -3032,43 +4880,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-17/08</t>
+24/08</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-18/08</t>
+25/08</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-19/08</t>
+26/08</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-20/08</t>
+27/08</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-21/08</t>
+28/08</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-22/08</t>
+29/08</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-23/08</t>
+30/08</t>
         </is>
       </c>
     </row>
@@ -3080,59 +4928,55 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
-        <is>
-          <t>MH007
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
@@ -3145,7 +4989,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
@@ -3154,27 +4998,27 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH005
-(Practice)
-Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
@@ -3184,22 +5028,85 @@
       <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="9" t="inlineStr">
+      <c r="H11" s="8" t="inlineStr">
         <is>
           <t>MH007
 (Theory)
-Room: LT1
-Lecturer: GV003</t>
+Room: LT3
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
-    <row r="12"/>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -3207,13 +5114,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3257,7 +5164,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 7 TIMETABLE (24/08/2026 - 30/08/2026)</t>
+          <t>WEEK 8 TIMETABLE (31/08/2026 - 06/09/2026)</t>
         </is>
       </c>
     </row>
@@ -3280,113 +5187,116 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-24/08</t>
+31/08</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-25/08</t>
+01/09</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-26/08</t>
+02/09</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-27/08</t>
+03/09</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-28/08</t>
+04/09</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-29/08</t>
+05/09</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-30/08</t>
+06/09</t>
         </is>
       </c>
     </row>
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="inlineStr"/>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH005
-(Practice)
-Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
@@ -3395,23 +5305,115 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
-    <row r="11"/>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH22IT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
@@ -3419,13 +5421,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3469,7 +5471,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 8 TIMETABLE (31/08/2026 - 06/09/2026)</t>
+          <t>WEEK 9 TIMETABLE (07/09/2026 - 13/09/2026)</t>
         </is>
       </c>
     </row>
@@ -3492,43 +5494,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-31/08</t>
+07/09</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-01/09</t>
+08/09</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-02/09</t>
+09/09</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-03/09</t>
+10/09</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-04/09</t>
+11/09</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-05/09</t>
+12/09</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-06/09</t>
+13/09</t>
         </is>
       </c>
     </row>
@@ -3540,52 +5542,55 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH2
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>MH014
+(Theory)
+Room: LT1
 Lecturer: GV002</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr"/>
       <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT1
+Lecturer: GV002</t>
+        </is>
+      </c>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
       <c r="J9" s="7" t="inlineStr"/>
@@ -3598,7 +5603,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
@@ -3607,16 +5612,16 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH005
-(Practice)
-Room: TH1
-Lecturer: GV002</t>
-        </is>
-      </c>
+      <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="60" customHeight="1">
@@ -3627,24 +5632,24 @@
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: TH3
-Lecturer: GV007</t>
-        </is>
-      </c>
+      <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>MH007
+(Theory)
+Room: LT3
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
@@ -3656,7 +5661,7 @@
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>DH22IT</t>
         </is>
       </c>
       <c r="C12" s="7" t="n">
@@ -3665,206 +5670,57 @@
       <c r="D12" s="7" t="inlineStr"/>
       <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
         <is>
           <t>MH007
 (Theory)
-Room: LT1
-Lecturer: GV003</t>
+Room: LT2
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
-    <row r="13"/>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MH008
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A2:J2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
-    <col width="25" customWidth="1" min="7" max="7"/>
-    <col width="25" customWidth="1" min="8" max="8"/>
-    <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>CANTHO UNIVERSITY SOFTWARE CENTER</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>TRUNG TÂM PHẦN MỀM ĐẠI HỌC CẦN THƠ</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Khu 3, Đại học Cần Thơ - 01 Lý Tự Trọng, TP Cần Thơ - Tel: 0292.3731072 &amp; Fax: 0292.3731071 - Email: cusc@ctu.edu.vn</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>WEEK 9 TIMETABLE (07/09/2026 - 13/09/2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="40" customHeight="1">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Time Slot</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>Class</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Students</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>Monday
-07/09</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>Tuesday
-08/09</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>Wednesday
-09/09</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>Thursday
-10/09</t>
-        </is>
-      </c>
-      <c r="H7" s="5" t="inlineStr">
-        <is>
-          <t>Friday
-11/09</t>
-        </is>
-      </c>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>Saturday
-12/09</t>
-        </is>
-      </c>
-      <c r="J7" s="5" t="inlineStr">
-        <is>
-          <t>Sunday
-13/09</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="60" customHeight="1">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>MH005
-(Theory)
-Room: LT2
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L1</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>MH007
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="I9" s="7" t="inlineStr"/>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10"/>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>

</xml_diff>